<commit_message>
JPD New Web Template changes
</commit_message>
<xml_diff>
--- a/src/assets/forms/ARN-Register.xlsx
+++ b/src/assets/forms/ARN-Register.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rahameda/Desktop/try/Mani/jpdglobalUI/src/assets/forms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rahameda/Desktop/try/rafik/jpd-global-ui-new/src/assets/forms/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="9240"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27180" windowHeight="10620"/>
   </bookViews>
   <sheets>
     <sheet name="Basic CSV template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Business type</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Business and trading website name</t>
+  </si>
+  <si>
+    <t>Date Of Birth</t>
+  </si>
+  <si>
+    <t>Registration Date</t>
   </si>
   <si>
     <t>Tax identification number in your home country</t>
@@ -66,7 +72,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +206,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.5"/>
+      <color rgb="FF4B4B4B"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -499,7 +520,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -542,11 +563,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -580,6 +604,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -646,7 +671,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -698,7 +723,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -900,24 +925,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -949,10 +980,21 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
         <v>10</v>
       </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="D2" s="1"/>
+      <c r="K2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>